<commit_message>
reformatted code, new errors classes. Trying to adapt the rescale function for further adapt of kernels. The 12 csv reformatted.
</commit_message>
<xml_diff>
--- a/csv_files/simulations data setup.xlsx
+++ b/csv_files/simulations data setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nie_k\Desktop\travail\RESEARCH\RESEARCH COHEN\Hawkes process Work\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA816A6D-6585-46F8-940E-0A72C5B340ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D25A0D-35C1-444D-B4D1-CB66A7F523B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="32">
   <si>
     <t>functions</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>super_smaller_12_first</t>
+  </si>
+  <si>
+    <t>change h to 1.75</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1136,61 +1139,89 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="14">
-        <v>120</v>
-      </c>
-      <c r="B23" s="16">
-        <v>6</v>
-      </c>
-      <c r="C23" s="16">
+      <c r="A23" s="6">
+        <v>120</v>
+      </c>
+      <c r="B23" s="7">
+        <v>12</v>
+      </c>
+      <c r="C23" s="7">
         <v>80</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="D23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="14">
+        <v>120</v>
+      </c>
+      <c r="B24" s="16">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16">
+        <v>80</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="I24" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1">
-      <c r="A24" s="10">
-        <v>120</v>
-      </c>
-      <c r="B24" s="11">
-        <v>6</v>
-      </c>
-      <c r="C24" s="11">
+    <row r="25" spans="1:9" ht="15" thickBot="1">
+      <c r="A25" s="10">
+        <v>120</v>
+      </c>
+      <c r="B25" s="11">
+        <v>12</v>
+      </c>
+      <c r="C25" s="11">
         <v>80</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="12" t="s">
+      <c r="D25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I25" s="13" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="D27" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done resimulating the pictures, and erase super_smaller_1_first.csv and super_smaller_1_second.csv because I am not using them.
</commit_message>
<xml_diff>
--- a/csv_files/simulations data setup.xlsx
+++ b/csv_files/simulations data setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nie_k\Desktop\travail\RESEARCH\RESEARCH COHEN\Hawkes process Work\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D25A0D-35C1-444D-B4D1-CB66A7F523B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F6A751-E7FF-4FD0-9EB7-C898ADDD721C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
   <si>
     <t>functions</t>
   </si>
@@ -75,9 +75,6 @@
     <t>NAN</t>
   </si>
   <si>
-    <t>super_smaller_1_first</t>
-  </si>
-  <si>
     <t>super_smaller_2_first</t>
   </si>
   <si>
@@ -121,6 +118,33 @@
   </si>
   <si>
     <t>change h to 1.75</t>
+  </si>
+  <si>
+    <t>super_1_second</t>
+  </si>
+  <si>
+    <t>super_2_second</t>
+  </si>
+  <si>
+    <t>super_3_second</t>
+  </si>
+  <si>
+    <t>super_4_second</t>
+  </si>
+  <si>
+    <t>super_smaller_2_second</t>
+  </si>
+  <si>
+    <t>super_smaller_3_second</t>
+  </si>
+  <si>
+    <t>super_smaller_4_second</t>
+  </si>
+  <si>
+    <t>super_smaller_12_second</t>
+  </si>
+  <si>
+    <t>super_smaller_12_third</t>
   </si>
 </sst>
 </file>
@@ -591,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="121" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -611,7 +635,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1">
       <c r="A1" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>0</v>
@@ -651,7 +675,7 @@
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -673,7 +697,7 @@
         <v>70</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
@@ -688,7 +712,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -702,7 +726,7 @@
         <v>70</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>9</v>
@@ -714,10 +738,10 @@
         <v>13</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -731,7 +755,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>9</v>
@@ -746,7 +770,7 @@
         <v>15</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -760,7 +784,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>9</v>
@@ -772,10 +796,10 @@
         <v>13</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -789,7 +813,7 @@
         <v>100</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>9</v>
@@ -804,7 +828,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -818,7 +842,7 @@
         <v>100</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>9</v>
@@ -830,10 +854,10 @@
         <v>13</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -862,7 +886,7 @@
         <v>15</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1">
@@ -888,15 +912,15 @@
         <v>13</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -907,31 +931,31 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="2">
-        <v>120</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3">
-        <v>70</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="A15" s="6">
+        <v>120</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7">
+        <v>80</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -940,10 +964,10 @@
         <v>120</v>
       </c>
       <c r="B16" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="7">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>8</v>
@@ -961,7 +985,7 @@
         <v>16</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -969,10 +993,10 @@
         <v>120</v>
       </c>
       <c r="B17" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="7">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>8</v>
@@ -998,10 +1022,10 @@
         <v>120</v>
       </c>
       <c r="B18" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="7">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>8</v>
@@ -1019,7 +1043,7 @@
         <v>17</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1027,19 +1051,19 @@
         <v>120</v>
       </c>
       <c r="B19" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" s="7">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>14</v>
@@ -1056,19 +1080,19 @@
         <v>120</v>
       </c>
       <c r="B20" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20" s="7">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>13</v>
@@ -1077,7 +1101,7 @@
         <v>18</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1085,143 +1109,85 @@
         <v>120</v>
       </c>
       <c r="B21" s="7">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C21" s="7">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="14">
+        <v>120</v>
+      </c>
+      <c r="B22" s="16">
         <v>12</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="C22" s="16">
+        <v>80</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="6">
-        <v>120</v>
-      </c>
-      <c r="B22" s="7">
-        <v>4</v>
-      </c>
-      <c r="C22" s="7">
-        <v>65</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="I22" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1">
+      <c r="A23" s="10">
+        <v>120</v>
+      </c>
+      <c r="B23" s="11">
+        <v>12</v>
+      </c>
+      <c r="C23" s="11">
+        <v>80</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="8" t="s">
+      <c r="E23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="6">
-        <v>120</v>
-      </c>
-      <c r="B23" s="7">
-        <v>12</v>
-      </c>
-      <c r="C23" s="7">
-        <v>80</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="14">
-        <v>120</v>
-      </c>
-      <c r="B24" s="16">
-        <v>12</v>
-      </c>
-      <c r="C24" s="16">
-        <v>80</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="9" t="s">
+      <c r="H23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="D25" s="16" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1">
-      <c r="A25" s="10">
-        <v>120</v>
-      </c>
-      <c r="B25" s="11">
-        <v>12</v>
-      </c>
-      <c r="C25" s="11">
-        <v>80</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="D27" s="16" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NEW parameters for l and h. Rounded the time estimation. Times used from data not from the files. I also created two files for simulation and drawing.
</commit_message>
<xml_diff>
--- a/csv_files/simulations data setup.xlsx
+++ b/csv_files/simulations data setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nie_k\Desktop\travail\RESEARCH\RESEARCH COHEN\Hawkes process Work\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F6A751-E7FF-4FD0-9EB7-C898ADDD721C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF428FF-92F9-4E17-94CC-103DC4CEA9B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="1800" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="121" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -918,7 +918,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="15" thickBot="1">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -931,31 +931,31 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="6">
-        <v>120</v>
-      </c>
-      <c r="B15" s="7">
+      <c r="A15" s="2">
+        <v>120</v>
+      </c>
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="3">
         <v>80</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="E15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I changed how the parameters are imported. I also solved a problem in ARMIJO (the todo I wrote a few comits ago)
</commit_message>
<xml_diff>
--- a/csv_files/simulations data setup.xlsx
+++ b/csv_files/simulations data setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nie_k\Desktop\travail\RESEARCH\RESEARCH COHEN\Hawkes process Work\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF428FF-92F9-4E17-94CC-103DC4CEA9B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6ABDF9-931D-43FE-9992-69A57490ECE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="1800" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13992" yWindow="3696" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="41">
   <si>
     <t>functions</t>
   </si>
@@ -117,9 +117,6 @@
     <t>super_smaller_12_first</t>
   </si>
   <si>
-    <t>change h to 1.75</t>
-  </si>
-  <si>
     <t>super_1_second</t>
   </si>
   <si>
@@ -145,6 +142,12 @@
   </si>
   <si>
     <t>super_smaller_12_third</t>
+  </si>
+  <si>
+    <t>super_0_first</t>
+  </si>
+  <si>
+    <t>super_0_second</t>
   </si>
 </sst>
 </file>
@@ -615,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -691,13 +694,13 @@
         <v>120</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
@@ -712,7 +715,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -720,13 +723,13 @@
         <v>120</v>
       </c>
       <c r="B5" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="7">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>9</v>
@@ -738,10 +741,10 @@
         <v>13</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -749,10 +752,10 @@
         <v>120</v>
       </c>
       <c r="B6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="7">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>21</v>
@@ -764,13 +767,13 @@
         <v>10</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -778,10 +781,10 @@
         <v>120</v>
       </c>
       <c r="B7" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="7">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>21</v>
@@ -796,10 +799,10 @@
         <v>13</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -807,10 +810,10 @@
         <v>120</v>
       </c>
       <c r="B8" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="7">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>21</v>
@@ -828,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -836,10 +839,10 @@
         <v>120</v>
       </c>
       <c r="B9" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="7">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>21</v>
@@ -854,10 +857,10 @@
         <v>13</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -865,19 +868,19 @@
         <v>120</v>
       </c>
       <c r="B10" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="7">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>14</v>
@@ -886,135 +889,135 @@
         <v>15</v>
       </c>
       <c r="I10" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6">
+        <v>120</v>
+      </c>
+      <c r="B11" s="7">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7">
+        <v>100</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="6">
+        <v>120</v>
+      </c>
+      <c r="B12" s="7">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1">
-      <c r="A11" s="10">
-        <v>120</v>
-      </c>
-      <c r="B11" s="11">
+    <row r="13" spans="1:9" ht="15" thickBot="1">
+      <c r="A13" s="10">
+        <v>120</v>
+      </c>
+      <c r="B13" s="11">
         <v>4</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C13" s="11">
         <v>65</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1">
-      <c r="A14" t="s">
+      <c r="I13" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="2">
-        <v>120</v>
-      </c>
-      <c r="B15" s="3">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="2">
+        <v>120</v>
+      </c>
+      <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C17" s="3">
         <v>80</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="E17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="6">
-        <v>120</v>
-      </c>
-      <c r="B16" s="7">
-        <v>2</v>
-      </c>
-      <c r="C16" s="7">
-        <v>80</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="6">
-        <v>120</v>
-      </c>
-      <c r="B17" s="7">
-        <v>3</v>
-      </c>
-      <c r="C17" s="7">
-        <v>100</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1022,10 +1025,10 @@
         <v>120</v>
       </c>
       <c r="B18" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="7">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>8</v>
@@ -1040,10 +1043,10 @@
         <v>13</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1051,19 +1054,19 @@
         <v>120</v>
       </c>
       <c r="B19" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="7">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>14</v>
@@ -1072,7 +1075,7 @@
         <v>15</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1080,28 +1083,28 @@
         <v>120</v>
       </c>
       <c r="B20" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="7">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1109,86 +1112,142 @@
         <v>120</v>
       </c>
       <c r="B21" s="7">
+        <v>4</v>
+      </c>
+      <c r="C21" s="7">
+        <v>65</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="7">
+      <c r="G21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="6">
+        <v>120</v>
+      </c>
+      <c r="B22" s="7">
+        <v>4</v>
+      </c>
+      <c r="C22" s="7">
+        <v>65</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="6">
+        <v>120</v>
+      </c>
+      <c r="B23" s="7">
+        <v>12</v>
+      </c>
+      <c r="C23" s="7">
         <v>80</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="14">
-        <v>120</v>
-      </c>
-      <c r="B22" s="16">
+      <c r="E23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="14">
+        <v>120</v>
+      </c>
+      <c r="B24" s="16">
         <v>12</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C24" s="16">
         <v>80</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D24" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="8" t="s">
+      <c r="E24" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I24" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1">
+      <c r="A25" s="10">
+        <v>120</v>
+      </c>
+      <c r="B25" s="11">
+        <v>12</v>
+      </c>
+      <c r="C25" s="11">
+        <v>80</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1">
-      <c r="A23" s="10">
-        <v>120</v>
-      </c>
-      <c r="B23" s="11">
-        <v>12</v>
-      </c>
-      <c r="C23" s="11">
-        <v>80</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="D25" s="16" t="s">
-        <v>30</v>
-      </c>
+    <row r="27" spans="1:9">
+      <c r="D27" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>